<commit_message>
contact us api integration done
</commit_message>
<xml_diff>
--- a/fileSample/plugsityBusinessInvite.xlsx
+++ b/fileSample/plugsityBusinessInvite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anilvishwakarma/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anil/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3AEB6B-FDEA-3F41-9BAD-3F72C85FF034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB092B72-DBAA-3848-BBAD-B39CF1B146D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16220" xr2:uid="{0A84970D-76F5-7E48-985D-D9BDD69879F8}"/>
+    <workbookView xWindow="780" yWindow="820" windowWidth="27640" windowHeight="16220" xr2:uid="{0A84970D-76F5-7E48-985D-D9BDD69879F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,27 +25,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>businessName</t>
   </si>
   <si>
-    <t>businessEmail</t>
-  </si>
-  <si>
-    <t>businessWebsite</t>
-  </si>
-  <si>
-    <t>businessPhoneNumber</t>
-  </si>
-  <si>
-    <t>businessAddress</t>
-  </si>
-  <si>
-    <t>businessSocialMedia</t>
-  </si>
-  <si>
     <t>sample</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>socialMedia</t>
+  </si>
+  <si>
+    <t>www.das.com</t>
+  </si>
+  <si>
+    <t>aqwe@dsa.com</t>
+  </si>
+  <si>
+    <t>www.sds.com</t>
+  </si>
+  <si>
+    <t>dsdf</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>samplhghe@sa.com</t>
+  </si>
+  <si>
+    <t>ryry</t>
   </si>
 </sst>
 </file>
@@ -69,10 +99,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFC77DBB"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -436,7 +466,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,33 +479,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D2">
         <v>99293992</v>
@@ -484,27 +514,101 @@
         <v>400101</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>99293992</v>
+      </c>
+      <c r="E3">
+        <v>400101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>99293992</v>
+      </c>
+      <c r="E4">
+        <v>400101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>99293992</v>
+      </c>
+      <c r="E5">
+        <v>400101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>99293992</v>
+      </c>
+      <c r="E6">
+        <v>400101</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="wfsd2@gmail.com" xr:uid="{3B9BACC0-F480-8044-8980-C06573F6CDB9}"/>
+    <hyperlink ref="A4" r:id="rId1" display="wfsd2@gmail.com" xr:uid="{7732C113-45A5-804F-B670-E1B7CBB70E84}"/>
+    <hyperlink ref="A5" r:id="rId2" display="wfsd2@gmail.com" xr:uid="{2F553952-B80E-6E44-AD87-F463B576B879}"/>
+    <hyperlink ref="A6" r:id="rId3" display="wfsd2@gmail.com" xr:uid="{F20EEB23-DFB2-E143-AD4C-0AD7ADA4F018}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{4527540B-E94D-3942-B316-02A316E946F1}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{063615FD-A242-6D41-A26E-86F0153075A0}"/>
+    <hyperlink ref="A2" r:id="rId6" xr:uid="{3B9BACC0-F480-8044-8980-C06573F6CDB9}"/>
+    <hyperlink ref="A3" r:id="rId7" xr:uid="{6DC8A8D6-8E38-AE49-B459-4F0DE551442C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>